<commit_message>
Added Column name validator
</commit_message>
<xml_diff>
--- a/TestApp/bin/Debug/net6.0-windows/Resources/np_teszt.xlsx
+++ b/TestApp/bin/Debug/net6.0-windows/Resources/np_teszt.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felhasználó\source\repos\TestApp\TestApp\bin\Debug\net6.0\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felhasználó\source\repos\TestApp\TestApp\bin\Debug\net6.0-windows\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97251953-BC62-4766-BEA5-DBBFD84ABEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04301C10-95C7-451B-9AC3-D79B4D874E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4019,7 +4019,7 @@
       <selection activeCell="H12" sqref="H12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
-      <autoFilter ref="A3:L77" xr:uid="{0F6A80CB-E5DF-49AC-ACF4-C299F0913FF6}"/>
+      <autoFilter ref="A3:L77" xr:uid="{1571C79A-BF66-43CA-92B7-6FF6E31FBBBC}"/>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -4036,7 +4036,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1200" sqref="A1200"/>
-      <selection pane="bottomLeft" activeCell="N11" sqref="N11"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15422,7 +15422,7 @@
       <selection pane="bottomLeft" activeCell="H77" sqref="H77"/>
       <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.35433070866141736" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
       <pageSetup paperSize="9" scale="53" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A4:AV400" xr:uid="{3EC639C8-CA95-46E0-ADCA-062B0A9094CD}">
+      <autoFilter ref="A4:AV400" xr:uid="{C7B7D1BE-2837-4CC3-ACE5-C1DF1CA711C7}">
         <filterColumn colId="6">
           <filters>
             <filter val="2019.06"/>
@@ -15930,7 +15930,7 @@
       <selection activeCell="L44" sqref="L44"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A41:N455" xr:uid="{80AE7C13-D2B1-406D-9144-B9700A957CC3}"/>
+      <autoFilter ref="A41:N455" xr:uid="{E38958B4-9035-45E2-AD3A-E11130F5B8AC}"/>
     </customSheetView>
   </customSheetViews>
   <dataValidations count="4">

</xml_diff>